<commit_message>
Update 5 Desember 2021
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>No.</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Waktu Hadir</t>
+  </si>
+  <si>
+    <t>Lingkungan</t>
   </si>
 </sst>
 </file>
@@ -416,24 +419,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,33 +450,36 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="9"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>